<commit_message>
Update files for new excel link
</commit_message>
<xml_diff>
--- a/docs/data/uk_la_future/1.0.6/uk_la_future.xlsx
+++ b/docs/data/uk_la_future/1.0.6/uk_la_future.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8723" uniqueCount="4504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8691" uniqueCount="4503">
   <si>
     <t>Dataset</t>
   </si>
@@ -13513,22 +13513,19 @@
     <t>No</t>
   </si>
   <si>
-    <t>[, ]</t>
-  </si>
-  <si>
-    <t>[, ', N, o, r, t, h, e, r, n,  , I, r, e, l, a, n, d, ', ,,  , ', S, c, o, t, l, a, n, d, ', ,,  , ', E, n, g, l, a, n, d, ', ,,  , ', W, a, l, e, s, ', ]</t>
-  </si>
-  <si>
-    <t>[, ', N, I, D, ', ,,  , ', S, C, O, ', ,,  , ', N, M, D, ', ,,  , ', W, P, A, ', ,,  , ', U, A, ', ,,  , ', L, B, O, ', ,,  , ', M, D, ', ,,  , ', C, T, Y, ', ,,  , ', C, O, M, B, ', ,,  , ', S, R, A, ', ,,  , ', C, C, ', ]</t>
-  </si>
-  <si>
-    <t>[, ', N, I,  , d, i, s, t, r, i, c, t, ', ,,  , ', S, c, o, t, t, i, s, h,  , u, n, i, t, a, r, y,  , a, u, t, h, o, r, i, t, y, ', ,,  , ', N, o, n, -, m, e, t, r, o, p, o, l, i, t, a, n,  , d, i, s, t, r, i, c, t, ', ,,  , ', W, e, l, s, h,  , u, n, i, t, a, r, y,  , a, u, t, h, o, r, i, t, y, ', ,,  , ', U, n, i, t, a, r, y,  , a, u, t, h, o, r, i, t, y, ', ,,  , ', L, o, n, d, o, n,  , b, o, r, o, u, g, h, ', ,,  , ', M, e, t, r, o, p, o, l, i, t, a, n,  , d, i, s, t, r, i, c, t, ', ,,  , ', C, o, u, n, t, y, ', ,,  , ', C, o, m, b, i, n, e, d,  , a, u, t, h, o, r, i, t, y, ', ,,  , ', S, t, r, a, t, e, g, i, c,  , R, e, g, i, o, n, a, l,  , A, u, t, h, o, r, i, t, y, ', ,,  , ', C, i, t, y,  , c, o, r, p, o, r, a, t, i, o, n, ', ]</t>
-  </si>
-  <si>
-    <t>[, T, r, u, e, ,,  , F, a, l, s, e, ]</t>
-  </si>
-  <si>
-    <t>[, ', n, i,  , d, i, s, t, r, i, c, t, ', ,,  , ', u, n, i, t, a, r, y, ', ,,  , ', l, o, w, e, r,  , t, i, e, r, ', ,,  , ', u, p, p, e, r,  , t, i, e, r, ', ,,  , ', c, o, m, b, i, n, e, d, ', ]</t>
+    <t>Northern Ireland, Scotland, England, Wales</t>
+  </si>
+  <si>
+    <t>NID, SCO, NMD, WPA, UA, LBO, MD, CTY, COMB, SRA, CC</t>
+  </si>
+  <si>
+    <t>NI district, Scottish unitary authority, Non-metropolitan district, Welsh unitary authority, Unitary authority, London borough, Metropolitan district, County, Combined authority, Strategic Regional Authority, City corporation</t>
+  </si>
+  <si>
+    <t>True, False</t>
+  </si>
+  <si>
+    <t>ni district, unitary, lower tier, upper tier, combined</t>
   </si>
 </sst>
 </file>
@@ -54369,7 +54366,7 @@
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="110.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="749.7109375" customWidth="1"/>
+    <col min="6" max="6" width="229.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -54408,9 +54405,6 @@
       <c r="E2" t="s">
         <v>4496</v>
       </c>
-      <c r="F2" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -54428,9 +54422,6 @@
       <c r="E3" t="s">
         <v>4496</v>
       </c>
-      <c r="F3" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -54448,9 +54439,6 @@
       <c r="E4" t="s">
         <v>4497</v>
       </c>
-      <c r="F4" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -54468,9 +54456,6 @@
       <c r="E5" t="s">
         <v>4497</v>
       </c>
-      <c r="F5" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -54488,9 +54473,6 @@
       <c r="E6" t="s">
         <v>4497</v>
       </c>
-      <c r="F6" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
@@ -54508,9 +54490,6 @@
       <c r="E7" t="s">
         <v>4497</v>
       </c>
-      <c r="F7" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -54528,9 +54507,6 @@
       <c r="E8" t="s">
         <v>4497</v>
       </c>
-      <c r="F8" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -54549,7 +54525,7 @@
         <v>4497</v>
       </c>
       <c r="F9" t="s">
-        <v>4499</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -54568,9 +54544,6 @@
       <c r="E10" t="s">
         <v>4497</v>
       </c>
-      <c r="F10" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -54589,7 +54562,7 @@
         <v>4497</v>
       </c>
       <c r="F11" t="s">
-        <v>4500</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -54609,7 +54582,7 @@
         <v>4497</v>
       </c>
       <c r="F12" t="s">
-        <v>4501</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -54628,9 +54601,6 @@
       <c r="E13" t="s">
         <v>4497</v>
       </c>
-      <c r="F13" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -54648,9 +54618,6 @@
       <c r="E14" t="s">
         <v>4497</v>
       </c>
-      <c r="F14" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -54668,9 +54635,6 @@
       <c r="E15" t="s">
         <v>4496</v>
       </c>
-      <c r="F15" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -54688,9 +54652,6 @@
       <c r="E16" t="s">
         <v>4497</v>
       </c>
-      <c r="F16" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
@@ -54708,9 +54669,6 @@
       <c r="E17" t="s">
         <v>4497</v>
       </c>
-      <c r="F17" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
@@ -54729,7 +54687,7 @@
         <v>4497</v>
       </c>
       <c r="F18" t="s">
-        <v>4502</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -54748,9 +54706,6 @@
       <c r="E19" t="s">
         <v>4497</v>
       </c>
-      <c r="F19" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
@@ -54768,9 +54723,6 @@
       <c r="E20" t="s">
         <v>4497</v>
       </c>
-      <c r="F20" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
@@ -54788,9 +54740,6 @@
       <c r="E21" t="s">
         <v>4497</v>
       </c>
-      <c r="F21" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
@@ -54808,9 +54757,6 @@
       <c r="E22" t="s">
         <v>4497</v>
       </c>
-      <c r="F22" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -54828,9 +54774,6 @@
       <c r="E23" t="s">
         <v>4497</v>
       </c>
-      <c r="F23" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
@@ -54848,9 +54791,6 @@
       <c r="E24" t="s">
         <v>4497</v>
       </c>
-      <c r="F24" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
@@ -54868,9 +54808,6 @@
       <c r="E25" t="s">
         <v>4497</v>
       </c>
-      <c r="F25" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
@@ -54888,9 +54825,6 @@
       <c r="E26" t="s">
         <v>4497</v>
       </c>
-      <c r="F26" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
@@ -54908,9 +54842,6 @@
       <c r="E27" t="s">
         <v>4497</v>
       </c>
-      <c r="F27" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
@@ -54928,9 +54859,6 @@
       <c r="E28" t="s">
         <v>4497</v>
       </c>
-      <c r="F28" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
@@ -54949,7 +54877,7 @@
         <v>4497</v>
       </c>
       <c r="F29" t="s">
-        <v>4503</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -54969,7 +54897,7 @@
         <v>4497</v>
       </c>
       <c r="F30" t="s">
-        <v>4502</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -54988,9 +54916,6 @@
       <c r="E31" t="s">
         <v>4497</v>
       </c>
-      <c r="F31" t="s">
-        <v>4498</v>
-      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
@@ -55008,11 +54933,8 @@
       <c r="E32" t="s">
         <v>4497</v>
       </c>
-      <c r="F32" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -55028,11 +54950,8 @@
       <c r="E33" t="s">
         <v>4497</v>
       </c>
-      <c r="F33" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -55048,11 +54967,8 @@
       <c r="E34" t="s">
         <v>4497</v>
       </c>
-      <c r="F34" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -55068,11 +54984,8 @@
       <c r="E35" t="s">
         <v>4497</v>
       </c>
-      <c r="F35" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -55088,11 +55001,8 @@
       <c r="E36" t="s">
         <v>4497</v>
       </c>
-      <c r="F36" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -55108,11 +55018,8 @@
       <c r="E37" t="s">
         <v>4497</v>
       </c>
-      <c r="F37" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -55128,11 +55035,8 @@
       <c r="E38" t="s">
         <v>4497</v>
       </c>
-      <c r="F38" t="s">
-        <v>4498</v>
-      </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -55147,9 +55051,6 @@
       </c>
       <c r="E39" t="s">
         <v>4497</v>
-      </c>
-      <c r="F39" t="s">
-        <v>4498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>